<commit_message>
correct ordering in case event fields of MultiPage
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/GenericDefinitionFile.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/GenericDefinitionFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/HMCTS/DEVLAB/WS/STS_HMCTS/CCD/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E871657-F79C-BE48-B405-CFCFDB1DCB06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4DAAC2-F1FA-824A-B5FD-642193D2B8EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15000" yWindow="-12820" windowWidth="33300" windowHeight="13440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4800" yWindow="-13440" windowWidth="33300" windowHeight="13440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -13890,8 +13890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14738,7 +14738,7 @@
         <v>630</v>
       </c>
       <c r="J21" s="94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K21" s="95"/>
       <c r="L21" s="95"/>
@@ -14816,7 +14816,7 @@
         <v>634</v>
       </c>
       <c r="J23" s="94">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K23" s="95"/>
       <c r="L23" s="95"/>

</xml_diff>